<commit_message>
add new acceptance file with requirments in english
</commit_message>
<xml_diff>
--- a/system design/דרישות.xlsx
+++ b/system design/דרישות.xlsx
@@ -5,12 +5,12 @@
   <workbookPr defaultThemeVersion="202300"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/andreibeloziorove/Desktop/"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/andreibeloziorove/Desktop/middleProjectBistro_16/system design/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{FADF2FDB-8ED2-1F45-BCE0-1DA1D1966959}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{1686A34B-075E-2147-AB4D-1AAFC1C90068}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="1340" yWindow="820" windowWidth="67260" windowHeight="27780" xr2:uid="{37C7EEAC-922F-7B4D-9CDB-A627DB64C0B8}"/>
+    <workbookView xWindow="200" yWindow="880" windowWidth="14820" windowHeight="18560" xr2:uid="{37C7EEAC-922F-7B4D-9CDB-A627DB64C0B8}"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
@@ -36,7 +36,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="121" uniqueCount="64">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="122" uniqueCount="65">
   <si>
     <t xml:space="preserve">דרישה </t>
   </si>
@@ -137,9 +137,6 @@
     <t>המערכת תציע מקום פנוי קרוב ביותר למעוד הזמנה</t>
   </si>
   <si>
-    <t xml:space="preserve">הצעת מקום צקרה אם אין מקום פנוי בזמן השלקוח רוצה או שאין שולחן פנוי בגודל שהוא רוצה </t>
-  </si>
-  <si>
     <t>זמנים קרובים הם באותו ים מטווח של משעה ועד סגירת מסעדה באותו יום</t>
   </si>
   <si>
@@ -191,9 +188,6 @@
     <t>המערכת תאפשר פינוי שולחן</t>
   </si>
   <si>
-    <t xml:space="preserve">פינוי שולחן דורש שהתשלום יצבצע לפניו </t>
-  </si>
-  <si>
     <t xml:space="preserve">נציג מסעדה ומנהל יכולים לצפות ברשימת המתנה ופירוט כל הזמנות, רשימת סועדים, ומנויים </t>
   </si>
   <si>
@@ -228,6 +222,15 @@
   </si>
   <si>
     <t>המידע הנשמר עבור כל הזמנה היא: קוד הזמנה, תאריך הזמנה, שעת הזמנה, מספר סועדים, האם המזמין הגיע בפועלת וסיים</t>
+  </si>
+  <si>
+    <t xml:space="preserve">הצעת מקום תקרה אם אין מקום פנוי בזמן השלקוח רוצה או שאין שולחן פנוי בגודל שהוא רוצה </t>
+  </si>
+  <si>
+    <t xml:space="preserve">פינוי שולחן דורש שהתשלום יתבצע לפניו </t>
+  </si>
+  <si>
+    <t xml:space="preserve">המערכת תיאפשר בחירת תווח זמנים להנפקת דוחות </t>
   </si>
 </sst>
 </file>
@@ -250,7 +253,7 @@
       <scheme val="minor"/>
     </font>
   </fonts>
-  <fills count="4">
+  <fills count="5">
     <fill>
       <patternFill patternType="none"/>
     </fill>
@@ -269,6 +272,12 @@
         <bgColor indexed="65"/>
       </patternFill>
     </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="FFFFFF00"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
   </fills>
   <borders count="1">
     <border>
@@ -284,7 +293,7 @@
     <xf numFmtId="0" fontId="1" fillId="2" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
     <xf numFmtId="0" fontId="1" fillId="3" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
   </cellStyleXfs>
-  <cellXfs count="4">
+  <cellXfs count="5">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
@@ -295,6 +304,7 @@
     <xf numFmtId="0" fontId="1" fillId="3" borderId="0" xfId="2" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
+    <xf numFmtId="0" fontId="0" fillId="4" borderId="0" xfId="0" applyFill="1"/>
   </cellXfs>
   <cellStyles count="3">
     <cellStyle name="40% - Accent1" xfId="1" builtinId="31"/>
@@ -633,8 +643,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{F0FCF7D1-2845-CB43-B6B4-F122C4F29DF2}">
   <dimension ref="A1:F31"/>
   <sheetViews>
-    <sheetView tabSelected="1" zoomScale="224" zoomScaleNormal="150" workbookViewId="0">
-      <selection activeCell="B24" sqref="B24"/>
+    <sheetView tabSelected="1" topLeftCell="C9" zoomScale="141" zoomScaleNormal="150" workbookViewId="0">
+      <selection activeCell="E17" sqref="E17"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
@@ -658,7 +668,7 @@
       <c r="A2" s="2" t="s">
         <v>3</v>
       </c>
-      <c r="B2" t="s">
+      <c r="B2" s="4" t="s">
         <v>2</v>
       </c>
       <c r="C2">
@@ -667,8 +677,8 @@
       <c r="D2" s="3" t="s">
         <v>4</v>
       </c>
-      <c r="E2" t="s">
-        <v>34</v>
+      <c r="E2" s="4" t="s">
+        <v>33</v>
       </c>
       <c r="F2">
         <v>31</v>
@@ -678,7 +688,7 @@
       <c r="A3" s="3" t="s">
         <v>4</v>
       </c>
-      <c r="B3" t="s">
+      <c r="B3" s="4" t="s">
         <v>8</v>
       </c>
       <c r="C3">
@@ -687,8 +697,8 @@
       <c r="D3" s="2" t="s">
         <v>3</v>
       </c>
-      <c r="E3" t="s">
-        <v>35</v>
+      <c r="E3" s="4" t="s">
+        <v>34</v>
       </c>
       <c r="F3">
         <v>32</v>
@@ -707,8 +717,8 @@
       <c r="D4" s="3" t="s">
         <v>4</v>
       </c>
-      <c r="E4" t="s">
-        <v>36</v>
+      <c r="E4" s="4" t="s">
+        <v>35</v>
       </c>
       <c r="F4">
         <v>33</v>
@@ -727,8 +737,8 @@
       <c r="D5" s="3" t="s">
         <v>4</v>
       </c>
-      <c r="E5" t="s">
-        <v>37</v>
+      <c r="E5" s="4" t="s">
+        <v>36</v>
       </c>
       <c r="F5">
         <v>34</v>
@@ -747,8 +757,8 @@
       <c r="D6" s="2" t="s">
         <v>3</v>
       </c>
-      <c r="E6" t="s">
-        <v>39</v>
+      <c r="E6" s="4" t="s">
+        <v>38</v>
       </c>
       <c r="F6">
         <v>35</v>
@@ -768,7 +778,7 @@
         <v>3</v>
       </c>
       <c r="E7" t="s">
-        <v>38</v>
+        <v>37</v>
       </c>
       <c r="F7">
         <v>36</v>
@@ -787,8 +797,8 @@
       <c r="D8" s="3" t="s">
         <v>4</v>
       </c>
-      <c r="E8" t="s">
-        <v>41</v>
+      <c r="E8" s="4" t="s">
+        <v>40</v>
       </c>
       <c r="F8">
         <v>37</v>
@@ -807,8 +817,8 @@
       <c r="D9" s="3" t="s">
         <v>4</v>
       </c>
-      <c r="E9" t="s">
-        <v>40</v>
+      <c r="E9" s="4" t="s">
+        <v>39</v>
       </c>
       <c r="F9">
         <v>38</v>
@@ -827,8 +837,8 @@
       <c r="D10" s="3" t="s">
         <v>4</v>
       </c>
-      <c r="E10" t="s">
-        <v>42</v>
+      <c r="E10" s="4" t="s">
+        <v>41</v>
       </c>
       <c r="F10">
         <v>39</v>
@@ -847,8 +857,8 @@
       <c r="D11" s="2" t="s">
         <v>3</v>
       </c>
-      <c r="E11" t="s">
-        <v>43</v>
+      <c r="E11" s="4" t="s">
+        <v>42</v>
       </c>
       <c r="F11">
         <v>40</v>
@@ -867,8 +877,8 @@
       <c r="D12" s="3" t="s">
         <v>4</v>
       </c>
-      <c r="E12" t="s">
-        <v>44</v>
+      <c r="E12" s="4" t="s">
+        <v>43</v>
       </c>
       <c r="F12">
         <v>41</v>
@@ -887,8 +897,8 @@
       <c r="D13" s="2" t="s">
         <v>3</v>
       </c>
-      <c r="E13" t="s">
-        <v>45</v>
+      <c r="E13" s="4" t="s">
+        <v>44</v>
       </c>
       <c r="F13">
         <v>42</v>
@@ -898,7 +908,7 @@
       <c r="A14" s="2" t="s">
         <v>3</v>
       </c>
-      <c r="B14" t="s">
+      <c r="B14" s="4" t="s">
         <v>16</v>
       </c>
       <c r="C14">
@@ -907,8 +917,8 @@
       <c r="D14" s="3" t="s">
         <v>4</v>
       </c>
-      <c r="E14" t="s">
-        <v>46</v>
+      <c r="E14" s="4" t="s">
+        <v>45</v>
       </c>
       <c r="F14">
         <v>43</v>
@@ -918,8 +928,8 @@
       <c r="A15" s="3" t="s">
         <v>4</v>
       </c>
-      <c r="B15" t="s">
-        <v>63</v>
+      <c r="B15" s="4" t="s">
+        <v>61</v>
       </c>
       <c r="C15">
         <v>14</v>
@@ -927,8 +937,8 @@
       <c r="D15" s="2" t="s">
         <v>3</v>
       </c>
-      <c r="E15" t="s">
-        <v>47</v>
+      <c r="E15" s="4" t="s">
+        <v>46</v>
       </c>
       <c r="F15">
         <v>44</v>
@@ -938,7 +948,7 @@
       <c r="A16" s="3" t="s">
         <v>4</v>
       </c>
-      <c r="B16" t="s">
+      <c r="B16" s="4" t="s">
         <v>23</v>
       </c>
       <c r="C16">
@@ -947,8 +957,8 @@
       <c r="D16" s="3" t="s">
         <v>4</v>
       </c>
-      <c r="E16" t="s">
-        <v>48</v>
+      <c r="E16" s="4" t="s">
+        <v>47</v>
       </c>
       <c r="F16">
         <v>45</v>
@@ -958,7 +968,7 @@
       <c r="A17" s="3" t="s">
         <v>4</v>
       </c>
-      <c r="B17" t="s">
+      <c r="B17" s="4" t="s">
         <v>24</v>
       </c>
       <c r="C17">
@@ -967,8 +977,8 @@
       <c r="D17" s="3" t="s">
         <v>4</v>
       </c>
-      <c r="E17" t="s">
-        <v>49</v>
+      <c r="E17" s="4" t="s">
+        <v>48</v>
       </c>
       <c r="F17">
         <v>46</v>
@@ -987,8 +997,8 @@
       <c r="D18" s="2" t="s">
         <v>3</v>
       </c>
-      <c r="E18" t="s">
-        <v>50</v>
+      <c r="E18" s="4" t="s">
+        <v>49</v>
       </c>
       <c r="F18">
         <v>47</v>
@@ -1007,8 +1017,8 @@
       <c r="D19" s="3" t="s">
         <v>4</v>
       </c>
-      <c r="E19" t="s">
-        <v>51</v>
+      <c r="E19" s="4" t="s">
+        <v>63</v>
       </c>
       <c r="F19">
         <v>48</v>
@@ -1028,7 +1038,7 @@
         <v>3</v>
       </c>
       <c r="E20" t="s">
-        <v>52</v>
+        <v>50</v>
       </c>
       <c r="F20">
         <v>49</v>
@@ -1048,7 +1058,7 @@
         <v>3</v>
       </c>
       <c r="E21" t="s">
-        <v>53</v>
+        <v>51</v>
       </c>
       <c r="F21">
         <v>50</v>
@@ -1058,7 +1068,7 @@
       <c r="A22" s="2" t="s">
         <v>3</v>
       </c>
-      <c r="B22" t="s">
+      <c r="B22" s="4" t="s">
         <v>22</v>
       </c>
       <c r="C22">
@@ -1068,7 +1078,7 @@
         <v>3</v>
       </c>
       <c r="E22" t="s">
-        <v>54</v>
+        <v>52</v>
       </c>
       <c r="F22">
         <v>51</v>
@@ -1078,7 +1088,7 @@
       <c r="A23" s="2" t="s">
         <v>3</v>
       </c>
-      <c r="B23" t="s">
+      <c r="B23" s="4" t="s">
         <v>25</v>
       </c>
       <c r="C23">
@@ -1088,7 +1098,7 @@
         <v>3</v>
       </c>
       <c r="E23" t="s">
-        <v>55</v>
+        <v>53</v>
       </c>
       <c r="F23">
         <v>52</v>
@@ -1098,7 +1108,7 @@
       <c r="A24" s="2" t="s">
         <v>3</v>
       </c>
-      <c r="B24" t="s">
+      <c r="B24" s="4" t="s">
         <v>26</v>
       </c>
       <c r="C24">
@@ -1108,7 +1118,7 @@
         <v>3</v>
       </c>
       <c r="E24" t="s">
-        <v>56</v>
+        <v>54</v>
       </c>
       <c r="F24">
         <v>53</v>
@@ -1118,7 +1128,7 @@
       <c r="A25" s="3" t="s">
         <v>4</v>
       </c>
-      <c r="B25" t="s">
+      <c r="B25" s="4" t="s">
         <v>27</v>
       </c>
       <c r="C25">
@@ -1127,8 +1137,8 @@
       <c r="D25" s="2" t="s">
         <v>3</v>
       </c>
-      <c r="E25" t="s">
-        <v>57</v>
+      <c r="E25" s="4" t="s">
+        <v>55</v>
       </c>
       <c r="F25">
         <v>54</v>
@@ -1138,7 +1148,7 @@
       <c r="A26" s="3" t="s">
         <v>4</v>
       </c>
-      <c r="B26" t="s">
+      <c r="B26" s="4" t="s">
         <v>28</v>
       </c>
       <c r="C26">
@@ -1148,7 +1158,7 @@
         <v>4</v>
       </c>
       <c r="E26" t="s">
-        <v>58</v>
+        <v>56</v>
       </c>
       <c r="F26">
         <v>55</v>
@@ -1158,7 +1168,7 @@
       <c r="A27" s="3" t="s">
         <v>4</v>
       </c>
-      <c r="B27" t="s">
+      <c r="B27" s="4" t="s">
         <v>29</v>
       </c>
       <c r="C27">
@@ -1167,8 +1177,8 @@
       <c r="D27" s="2" t="s">
         <v>3</v>
       </c>
-      <c r="E27" t="s">
-        <v>59</v>
+      <c r="E27" s="4" t="s">
+        <v>57</v>
       </c>
       <c r="F27">
         <v>56</v>
@@ -1178,7 +1188,7 @@
       <c r="A28" s="3" t="s">
         <v>4</v>
       </c>
-      <c r="B28" t="s">
+      <c r="B28" s="4" t="s">
         <v>30</v>
       </c>
       <c r="C28">
@@ -1188,7 +1198,7 @@
         <v>3</v>
       </c>
       <c r="E28" t="s">
-        <v>60</v>
+        <v>58</v>
       </c>
       <c r="F28">
         <v>57</v>
@@ -1198,7 +1208,7 @@
       <c r="A29" s="2" t="s">
         <v>3</v>
       </c>
-      <c r="B29" t="s">
+      <c r="B29" s="4" t="s">
         <v>31</v>
       </c>
       <c r="C29">
@@ -1207,8 +1217,8 @@
       <c r="D29" s="3" t="s">
         <v>4</v>
       </c>
-      <c r="E29" t="s">
-        <v>61</v>
+      <c r="E29" s="4" t="s">
+        <v>59</v>
       </c>
       <c r="F29">
         <v>58</v>
@@ -1218,7 +1228,7 @@
       <c r="A30" s="2" t="s">
         <v>3</v>
       </c>
-      <c r="B30" t="s">
+      <c r="B30" s="4" t="s">
         <v>32</v>
       </c>
       <c r="C30">
@@ -1228,7 +1238,7 @@
         <v>3</v>
       </c>
       <c r="E30" t="s">
-        <v>62</v>
+        <v>60</v>
       </c>
       <c r="F30">
         <v>59</v>
@@ -1238,11 +1248,14 @@
       <c r="A31" s="3" t="s">
         <v>4</v>
       </c>
-      <c r="B31" t="s">
-        <v>33</v>
+      <c r="B31" s="4" t="s">
+        <v>62</v>
       </c>
       <c r="C31">
         <v>30</v>
+      </c>
+      <c r="E31" s="4" t="s">
+        <v>64</v>
       </c>
     </row>
   </sheetData>

</xml_diff>